<commit_message>
Final changes to PCB design. Sent to order
</commit_message>
<xml_diff>
--- a/Altium Board Designs/STM32_display_test_board/Project Outputs for STM32_display_test_board/BOM/Bill of Materials-STM32_display_test_board.xlsx
+++ b/Altium Board Designs/STM32_display_test_board/Project Outputs for STM32_display_test_board/BOM/Bill of Materials-STM32_display_test_board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walke\repos\circuits-2024\Altium Board Designs\STM32_display_test_board\Project Outputs for STM32_display_test_board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{249C03BD-3362-4F9D-AF19-5732DB284B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97C6B7B1-658C-4E89-82C3-FC59861C2B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="84" windowWidth="7500" windowHeight="9024" xr2:uid="{0B1DDB0C-A43A-437D-A77D-54CE1403E74D}"/>
+    <workbookView xWindow="2124" yWindow="3192" windowWidth="10740" windowHeight="9024" xr2:uid="{FE4F92F4-5620-4504-849E-B63820EE0505}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-STM32_display" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="172">
   <si>
     <t>Line #</t>
   </si>
@@ -346,15 +346,6 @@
   </si>
   <si>
     <t>J3</t>
-  </si>
-  <si>
-    <t>Global Connector Technology</t>
-  </si>
-  <si>
-    <t>USB4110-GF-A</t>
-  </si>
-  <si>
-    <t>71AJ9394</t>
   </si>
   <si>
     <t>HyTech CAN Connector</t>
@@ -943,7 +934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{949497EC-9FE1-472D-8D15-5DC8595CEE67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ADB58A-558C-481D-A64D-ADC887CF51B8}">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1062,7 +1053,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1098,7 +1091,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1134,7 +1129,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1170,7 +1167,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1206,7 +1205,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1303,9 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
@@ -1330,7 +1333,9 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1363,9 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>63</v>
       </c>
@@ -1416,7 +1423,9 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>70</v>
       </c>
@@ -1444,7 +1453,9 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
@@ -1496,7 +1507,9 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>80</v>
       </c>
@@ -1532,7 +1545,9 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>86</v>
       </c>
@@ -1568,7 +1583,9 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>90</v>
       </c>
@@ -1628,7 +1645,9 @@
       <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>95</v>
       </c>
@@ -1677,38 +1696,24 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="1">
-        <v>1.34</v>
-      </c>
-      <c r="L23" s="1">
-        <v>1.34</v>
-      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -1722,24 +1727,26 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>18</v>
@@ -1748,7 +1755,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K25" s="1">
         <v>0.1</v>
@@ -1758,7 +1765,9 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
@@ -1766,7 +1775,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1775,7 +1784,7 @@
         <v>48</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>18</v>
@@ -1784,7 +1793,7 @@
         <v>30</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K26" s="1">
         <v>0.15659999999999999</v>
@@ -1798,22 +1807,22 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E27" s="1">
         <v>6</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>34</v>
@@ -1822,7 +1831,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K27" s="1">
         <v>0.72</v>
@@ -1836,22 +1845,22 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>50</v>
@@ -1862,24 +1871,26 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
+      <c r="A29" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>50</v>
@@ -1890,24 +1901,26 @@
       <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>50</v>
@@ -1922,22 +1935,22 @@
         <v>12</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>50</v>
@@ -1952,22 +1965,22 @@
         <v>12</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E32" s="1">
         <v>2</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>50</v>
@@ -1978,24 +1991,26 @@
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>50</v>
@@ -2010,22 +2025,22 @@
         <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E34" s="1">
         <v>2</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>50</v>
@@ -2040,22 +2055,22 @@
         <v>12</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E35" s="1">
         <v>2</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>50</v>
@@ -2066,24 +2081,26 @@
       <c r="L35" s="1"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
+      <c r="A36" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>50</v>
@@ -2094,24 +2111,26 @@
       <c r="L36" s="1"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B37" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>156</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>50</v>
@@ -2122,24 +2141,26 @@
       <c r="L37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
+      <c r="A38" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>34</v>
@@ -2148,7 +2169,7 @@
         <v>19</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K38" s="1">
         <v>0.75</v>
@@ -2158,24 +2179,26 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
+      <c r="A39" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="G39" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>50</v>
@@ -2186,15 +2209,17 @@
       <c r="L39" s="1"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
+      <c r="A40" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -2203,7 +2228,7 @@
         <v>24</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>18</v>
@@ -2212,7 +2237,7 @@
         <v>19</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K40" s="1">
         <v>1.87</v>
@@ -2222,15 +2247,17 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
+      <c r="A41" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -2244,24 +2271,26 @@
       <c r="L41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
+      <c r="A42" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B42" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>50</v>

</xml_diff>